<commit_message>
Layout dynamics w/ working product display
</commit_message>
<xml_diff>
--- a/Python/TestFile.xlsx
+++ b/Python/TestFile.xlsx
@@ -677,13 +677,67 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
+      <c r="A11" s="1" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2311090004</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Ji</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
+      <c r="A12" s="1" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Banana</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2311090004</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Ji</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n"/>
+      <c r="A13" s="1" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Berry </t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2311090004</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Ji</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>

</xml_diff>

<commit_message>
Scaleable Scroll, Quantity/Product Rework & Clear
</commit_message>
<xml_diff>
--- a/Python/TestFile.xlsx
+++ b/Python/TestFile.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -57,13 +59,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -740,13 +743,88 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n"/>
+      <c r="A14" s="1" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2311130005</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n"/>
+      <c r="A15" s="1" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Banana</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2311130005</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
+      <c r="A16" s="1" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Berry</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2311130005</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pineapple</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2311130005</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Front-end layer fully completed (R&D Branch)
</commit_message>
<xml_diff>
--- a/Python/TestFile.xlsx
+++ b/Python/TestFile.xlsx
@@ -602,28 +602,172 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n"/>
+      <c r="A7" s="1" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Yakuza Teriyaki</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2312200004</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Cherry M. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n"/>
+      <c r="A8" s="1" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Chicano Chili</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2312200004</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Cherry M. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
+      <c r="A9" s="1" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gangbanger Tuna</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2312200004</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Cherry M. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n"/>
+      <c r="A10" s="1" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Waddup Che&amp;Bac</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2312240005</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Fredrick James Paolo R. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
+      <c r="A11" s="1" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cheese Burger</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2312240005</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Fredrick James Paolo R. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
+      <c r="A12" s="1" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hardcore Overload </t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2312240005</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Fredrick James Paolo R. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n"/>
+      <c r="A13" s="1" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Waddup Che&amp;Bac</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2312240006</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Josefe Johnatan M. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n"/>
+      <c r="A14" s="1" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Chicano Chili</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2312240007</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Kristina Franchesca M. Gillego</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>

</xml_diff>

<commit_message>
All features implemented -- ready for android build
</commit_message>
<xml_diff>
--- a/Python/TestFile.xlsx
+++ b/Python/TestFile.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -519,18 +519,18 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45276</v>
+        <v>45284</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Watermelon</t>
+          <t>Gangbanger Tuna Burger</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>2312160001</v>
+        <v>2312240001</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -540,234 +540,126 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45279</v>
+        <v>45284</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gangbanger Tuna</t>
+          <t xml:space="preserve">Hardcore Overload </t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>2312190002</v>
+        <v>2312240001</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kristina Franchesca M. Gillego</t>
+          <t>Josefe Johnatan M. Gillego</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45280</v>
+        <v>45284</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Yakuza Teriyaki</t>
+          <t>Chicano Chili</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>2312200003</v>
+        <v>2312240002</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fredrick James Paolo R. Gillego</t>
+          <t>Josefe Johnatan M. Gillego</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45280</v>
+        <v>45284</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hardcore Overload</t>
+          <t>Rastaparay Veg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>2312200003</v>
+        <v>2312240003</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Fredrick James Paolo R. Gillego</t>
+          <t>Josefe Johnatan M. Gillego</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45280</v>
+        <v>45284</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yakuza Teriyaki</t>
+          <t>Chicano Chili</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>2312200004</v>
+        <v>2312240003</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Cherry M. Gillego</t>
+          <t>Josefe Johnatan M. Gillego</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45280</v>
+        <v>45284</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Chicano Chili</t>
+          <t xml:space="preserve">Hardcore Overload </t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>2312200004</v>
+        <v>2312240004</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Cherry M. Gillego</t>
+          <t>Jerome</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>45280</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Gangbanger Tuna</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2312200004</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Cherry M. Gillego</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Waddup Che&amp;Bac</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Fredrick James Paolo R. Gillego</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Cheese Burger</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Fredrick James Paolo R. Gillego</t>
-        </is>
-      </c>
+      <c r="A11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hardcore Overload </t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>6</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Fredrick James Paolo R. Gillego</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Waddup Che&amp;Bac</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2312240006</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Chicano Chili</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2312240007</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Kristina Franchesca M. Gillego</t>
-        </is>
-      </c>
+      <c r="A14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>

</xml_diff>

<commit_message>
Added a system to remove previous entries / minor UI reformat
</commit_message>
<xml_diff>
--- a/Python/TestFile.xlsx
+++ b/Python/TestFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5172" yWindow="1464" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2796" yWindow="408" windowWidth="17280" windowHeight="11736" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,8 +33,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +59,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -66,13 +78,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,20 +463,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="13.77734375" customWidth="1" min="1" max="1"/>
-    <col width="13.109375" customWidth="1" min="2" max="2"/>
+    <col width="22.5546875" customWidth="1" min="2" max="2"/>
     <col width="11.6640625" customWidth="1" min="3" max="3"/>
     <col width="14.77734375" customWidth="1" min="4" max="4"/>
     <col width="37.21875" customWidth="1" min="5" max="5"/>
-    <col width="12.109375" customWidth="1" min="6" max="6"/>
+    <col width="12.109375" customWidth="1" style="6" min="6" max="6"/>
+    <col width="17.88671875" customWidth="1" min="7" max="7"/>
     <col width="12.21875" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -493,6 +507,11 @@
           <t>Staff</t>
         </is>
       </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Total Revenue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -516,279 +535,48 @@
           <t>Placeholder</t>
         </is>
       </c>
+      <c r="G2" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Gangbanger Tuna Burger</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2312240001</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hardcore Overload </t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2312240001</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Chicano Chili</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2312240002</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Rastaparay Veg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2312240003</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Chicano Chili</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2312240003</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hardcore Overload </t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2312240004</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Jerome</t>
-        </is>
-      </c>
+      <c r="A8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Chicano Chili</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Gangbanger Tuna Burger</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Yakuza Teriyaki</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" t="n">
-        <v>2312240005</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Josefe Johnatan M. Gillego</t>
-        </is>
-      </c>
+      <c r="A11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Rastaparay Veg</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2312240006</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Cherry M. Gillego</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Gangbanger Tuna Burger</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>789</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2312240007</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Cherry M. Gillego</t>
-        </is>
-      </c>
+      <c r="A13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Yakuza Teriyaki</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>12</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2312240008</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Kristina Franchesca M. Gillego</t>
-        </is>
-      </c>
+      <c r="A14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>45284</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Chicano Chili</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2312240009</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Kristina Franchesca M. Gillego</t>
-        </is>
-      </c>
+      <c r="A15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
@@ -807,6 +595,30 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>